<commit_message>
Added Counts for Tony/Wilfred
</commit_message>
<xml_diff>
--- a/COUNTforSENG.xlsx
+++ b/COUNTforSENG.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16760" tabRatio="500"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
   <si>
     <t>Nested type count</t>
   </si>
@@ -65,12 +65,6 @@
     <t>Cancer Registry cgritt</t>
   </si>
   <si>
-    <t>IGV</t>
-  </si>
-  <si>
-    <t>Iridia</t>
-  </si>
-  <si>
     <t>re-do</t>
   </si>
   <si>
@@ -83,9 +77,6 @@
     <t>libSBOLj</t>
   </si>
   <si>
-    <t>intermine</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wilfredo's Projects </t>
   </si>
   <si>
@@ -132,6 +123,18 @@
   </si>
   <si>
     <t>Other Annotation</t>
+  </si>
+  <si>
+    <t>openCGA</t>
+  </si>
+  <si>
+    <t>genome-nexus</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>geneDB</t>
   </si>
 </sst>
 </file>
@@ -175,9 +178,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -468,401 +472,536 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" customWidth="1"/>
     <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="40" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+    </row>
+    <row r="2" spans="1:12" ht="40" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3" s="1">
-        <f>8+9+17+7+5+62+4+6+21</f>
-        <v>139</v>
-      </c>
-      <c r="D3" s="1">
-        <f>4+1+1+2</f>
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="C3" s="2">
+        <f>0+8+26+7+1+5+62+7+3+6+21</f>
+        <v>146</v>
+      </c>
+      <c r="D3" s="2">
+        <f>3+1</f>
         <v>4</v>
       </c>
-      <c r="F3" s="1">
-        <f>1+1+1+2+1</f>
-        <v>6</v>
-      </c>
-      <c r="G3">
+      <c r="E3" s="2">
+        <v>4</v>
+      </c>
+      <c r="F3" s="2">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
+      <c r="G3" s="2">
+        <f>32+119</f>
+        <v>151</v>
+      </c>
+      <c r="H3" s="2">
         <v>1</v>
       </c>
-      <c r="H3">
-        <f>5+1+1+2+1</f>
-        <v>10</v>
-      </c>
-      <c r="I3">
-        <f>33+1+3+1+1+1+69+4+18+7+10+8</f>
-        <v>156</v>
-      </c>
-      <c r="J3">
-        <v>15</v>
+      <c r="I3" s="2">
+        <f>40+18+7</f>
+        <v>65</v>
+      </c>
+      <c r="J3" s="2">
+        <v>23</v>
       </c>
       <c r="K3">
-        <f>23+18+5</f>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="1">
-        <v>0</v>
-      </c>
-      <c r="J4" s="1">
-        <v>0</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>0</v>
-      </c>
-      <c r="I5" s="1">
-        <v>0</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2">
+        <f>0+42+34+41+8+2+1+2+3+19</f>
+        <v>152</v>
+      </c>
+      <c r="D5" s="2">
+        <f>2</f>
+        <v>2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>1</v>
+      </c>
+      <c r="F5" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0</v>
+      </c>
+      <c r="I5" s="2">
+        <f>91+22+25</f>
+        <v>138</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>34</v>
       </c>
-      <c r="C6">
-        <f xml:space="preserve"> 99 + 74 + 17+79+51+107+78+285+153+7+128+409+367</f>
-        <v>1854</v>
-      </c>
-      <c r="D6">
-        <f>103+25+13+45+33+3+61</f>
-        <v>283</v>
-      </c>
-      <c r="E6">
+      <c r="C6" s="2">
+        <f>11+5+83+221+107+78+218+285+153+7+202+125+409+367</f>
+        <v>2271</v>
+      </c>
+      <c r="D6" s="2">
+        <f>297+27+23</f>
+        <v>347</v>
+      </c>
+      <c r="E6" s="2">
         <v>81</v>
       </c>
-      <c r="F6">
-        <f>7+5+3+16+9+13</f>
-        <v>53</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6">
-        <f>19+2+49+10+14+72+83+5+31</f>
-        <v>285</v>
-      </c>
-      <c r="I6">
-        <f>422+6+35+12+2+8+4+10+55+441+17+90+170+211+235+70+33</f>
-        <v>1821</v>
-      </c>
-      <c r="J6">
-        <v>106</v>
-      </c>
-      <c r="K6">
-        <f>423+23+342+52</f>
-        <v>840</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F6" s="2">
+        <f>9+24</f>
+        <v>33</v>
+      </c>
+      <c r="G6" s="2">
+        <f>94+71</f>
+        <v>165</v>
+      </c>
+      <c r="H6" s="2">
+        <v>133</v>
+      </c>
+      <c r="I6" s="2">
+        <f>558+170+211</f>
+        <v>939</v>
+      </c>
+      <c r="J6" s="2">
+        <v>127</v>
+      </c>
+      <c r="K6" s="2">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>67</v>
       </c>
-      <c r="C7">
-        <f xml:space="preserve"> 55 + 243 + 294 + 8 +217 +328+65+241+693+364+17+553+721+1580</f>
-        <v>5379</v>
-      </c>
-      <c r="D7">
-        <f>293+101+81+530+66+167</f>
-        <v>1238</v>
-      </c>
-      <c r="E7">
+      <c r="C7" s="2">
+        <f>53+2+243+847+65+241+546+693+364+17+689+272+721+1580</f>
+        <v>6333</v>
+      </c>
+      <c r="D7" s="2">
+        <f>780+101+81</f>
+        <v>962</v>
+      </c>
+      <c r="E7" s="2">
         <v>213</v>
       </c>
-      <c r="F7">
-        <f>16+4+14+11+8+9</f>
-        <v>62</v>
-      </c>
-      <c r="G7">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <f>13+37+8+8+4+74+4+4</f>
-        <v>152</v>
-      </c>
-      <c r="I7">
-        <f>1229+2+11+39+2+1+27+3+4+94+2234+12+411+617+813+603+138+77</f>
-        <v>6317</v>
-      </c>
-      <c r="J7">
-        <v>159</v>
-      </c>
-      <c r="K7">
-        <f>256+12+390+65</f>
-        <v>723</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="F7" s="2">
+        <f>16+29</f>
+        <v>45</v>
+      </c>
+      <c r="G7" s="2">
+        <f>439+72</f>
+        <v>511</v>
+      </c>
+      <c r="H7" s="2">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2">
+        <f>1412+617+840</f>
+        <v>2869</v>
+      </c>
+      <c r="J7" s="2">
+        <v>167</v>
+      </c>
+      <c r="K7" s="2">
+        <v>1129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2">
+        <f>18+4+538+1301+354+508+1244+959+382+242+1809+2058</f>
+        <v>9417</v>
+      </c>
+      <c r="D8" s="2">
+        <f>721+27+61</f>
+        <v>809</v>
+      </c>
+      <c r="E8" s="2">
+        <v>51</v>
+      </c>
+      <c r="F8" s="2">
+        <f>40+100</f>
+        <v>140</v>
+      </c>
+      <c r="G8" s="2">
+        <f>102+132</f>
+        <v>234</v>
+      </c>
+      <c r="H8" s="2">
+        <v>155</v>
+      </c>
+      <c r="I8" s="2">
+        <f>866+289+340</f>
+        <v>1495</v>
+      </c>
+      <c r="J8" s="2">
+        <v>210</v>
+      </c>
+      <c r="K8" s="2">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="2">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D10" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0</v>
+      </c>
+      <c r="F10" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>30</v>
       </c>
-      <c r="B8">
-        <v>27</v>
-      </c>
-      <c r="C8">
-        <v>40</v>
-      </c>
-      <c r="D8">
-        <v>1414</v>
-      </c>
-      <c r="E8">
-        <v>313</v>
-      </c>
-      <c r="F8">
-        <v>56</v>
-      </c>
-      <c r="G8">
-        <v>4</v>
-      </c>
-      <c r="H8">
-        <v>240</v>
-      </c>
-      <c r="I8">
-        <v>1018</v>
-      </c>
-      <c r="J8">
-        <v>227</v>
-      </c>
-      <c r="K8">
-        <f>196+9+239+46</f>
-        <v>490</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0</v>
+      </c>
+      <c r="F11" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2">
+        <v>0</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
+        <f>0</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>17</v>
+      </c>
+      <c r="K12" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
-      <c r="B13">
-        <v>28</v>
-      </c>
-      <c r="C13">
-        <v>67</v>
-      </c>
-      <c r="D13">
-        <v>14</v>
-      </c>
-      <c r="E13">
-        <v>34</v>
-      </c>
-      <c r="F13">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>8</v>
       </c>
       <c r="B14">
-        <f>B3/B6*100%</f>
-        <v>5.8823529411764705E-2</v>
+        <f>B3/B6*100</f>
+        <v>5.8823529411764701</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:F14" si="0">C3/C6*100%</f>
-        <v>7.4973031283710898E-2</v>
+        <f t="shared" ref="C14:K14" si="0">C3/C6*100</f>
+        <v>6.4288859533245271</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>2.8268551236749116E-2</v>
+        <v>1.1527377521613833</v>
       </c>
       <c r="E14">
         <f t="shared" si="0"/>
-        <v>4.9382716049382713E-2</v>
+        <v>4.9382716049382713</v>
       </c>
       <c r="F14">
-        <f>F3/F6*100%</f>
-        <v>0.11320754716981132</v>
+        <f t="shared" si="0"/>
+        <v>9.0909090909090917</v>
       </c>
       <c r="G14">
-        <f>G3/G6*100%</f>
-        <v>0.33333333333333331</v>
+        <f t="shared" si="0"/>
+        <v>91.515151515151516</v>
       </c>
       <c r="H14">
-        <f>H3/H6*100%</f>
-        <v>3.5087719298245612E-2</v>
+        <f t="shared" si="0"/>
+        <v>0.75187969924812026</v>
       </c>
       <c r="I14">
-        <f>I3/I6*100%</f>
-        <v>8.5667215815486003E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.9222577209797658</v>
       </c>
       <c r="J14">
-        <f>J3/J6*100%</f>
-        <v>0.14150943396226415</v>
+        <f t="shared" si="0"/>
+        <v>18.110236220472441</v>
       </c>
       <c r="K14">
-        <f>K3/K6*100%</f>
-        <v>5.4761904761904762E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>3.9416058394160585</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="E18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
+      <c r="F18" t="s">
         <v>21</v>
       </c>
-      <c r="D18" t="s">
+      <c r="G18" t="s">
         <v>22</v>
       </c>
-      <c r="E18" t="s">
+      <c r="H18" t="s">
         <v>23</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>24</v>
       </c>
-      <c r="G18" t="s">
+      <c r="J18" t="s">
         <v>25</v>
       </c>
-      <c r="H18" t="s">
+      <c r="K18" t="s">
         <v>26</v>
-      </c>
-      <c r="I18" t="s">
-        <v>27</v>
-      </c>
-      <c r="J18" t="s">
-        <v>28</v>
-      </c>
-      <c r="K18" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
@@ -1042,7 +1181,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -1077,7 +1216,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -1112,17 +1251,17 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
@@ -1133,6 +1272,46 @@
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
+      </c>
+      <c r="B30">
+        <f>B19/B22*100</f>
+        <v>3.322259136212625</v>
+      </c>
+      <c r="C30">
+        <f>C19/C22*100</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="D30">
+        <f t="shared" ref="D30:K30" si="1">D19/D22*100</f>
+        <v>2.9179810725552051</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="1"/>
+        <v>0.49507307088113484</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>20.512820512820511</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>34.972677595628419</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>15.476190476190476</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="1"/>
+        <v>13.247863247863249</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="1"/>
+        <v>4.2638777152051484</v>
+      </c>
+      <c r="K30">
+        <f t="shared" si="1"/>
+        <v>10.256410256410255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Counts for 10 projects
</commit_message>
<xml_diff>
--- a/COUNTforSENG.xlsx
+++ b/COUNTforSENG.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TonyTea/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simranbhattarai/Documents/GitHub/SENG300GROUP3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="7100" yWindow="460" windowWidth="21700" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Nested type count</t>
   </si>
@@ -135,6 +135,48 @@
   </si>
   <si>
     <t>geneDB</t>
+  </si>
+  <si>
+    <t>Types</t>
+  </si>
+  <si>
+    <t>Quartz Scheduler</t>
+  </si>
+  <si>
+    <t>Open EMRConect</t>
+  </si>
+  <si>
+    <t>Wallet</t>
+  </si>
+  <si>
+    <t>Secure Banking System</t>
+  </si>
+  <si>
+    <t>Calendar System</t>
+  </si>
+  <si>
+    <t>Time4J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voj </t>
+  </si>
+  <si>
+    <t>Core Flight Systm(CFS) and data Dictionary(CCDD) Utility</t>
+  </si>
+  <si>
+    <t>Dert</t>
+  </si>
+  <si>
+    <t>Hyper realistic zombie</t>
+  </si>
+  <si>
+    <t>Other Interface/class Decl (non nest/non local/non anon)</t>
+  </si>
+  <si>
+    <t>Annotation type Count</t>
+  </si>
+  <si>
+    <t>Import Declarations Count</t>
   </si>
 </sst>
 </file>
@@ -178,10 +220,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="N50" sqref="N50"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1314,6 +1365,286 @@
         <v>10.256410256410255</v>
       </c>
     </row>
+    <row r="33" spans="1:11" ht="96" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="4">
+        <v>71</v>
+      </c>
+      <c r="C34">
+        <v>22</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>20</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>4</v>
+      </c>
+      <c r="J34">
+        <v>14</v>
+      </c>
+      <c r="K34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="4">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="4">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="4">
+        <v>459</v>
+      </c>
+      <c r="C37">
+        <v>177</v>
+      </c>
+      <c r="D37">
+        <v>11</v>
+      </c>
+      <c r="E37">
+        <v>61</v>
+      </c>
+      <c r="F37">
+        <v>45</v>
+      </c>
+      <c r="G37">
+        <v>58</v>
+      </c>
+      <c r="H37">
+        <v>39</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>334</v>
+      </c>
+      <c r="K37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1181</v>
+      </c>
+      <c r="C38">
+        <v>542</v>
+      </c>
+      <c r="D38">
+        <v>3</v>
+      </c>
+      <c r="E38">
+        <v>112</v>
+      </c>
+      <c r="F38">
+        <v>116</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
+        <v>165</v>
+      </c>
+      <c r="I38">
+        <v>117</v>
+      </c>
+      <c r="J38">
+        <v>1088</v>
+      </c>
+      <c r="K38">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="4">
+        <v>517</v>
+      </c>
+      <c r="C39">
+        <v>78</v>
+      </c>
+      <c r="D39">
+        <v>27</v>
+      </c>
+      <c r="E39">
+        <v>311</v>
+      </c>
+      <c r="F39">
+        <v>62</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>74</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
+        <v>190</v>
+      </c>
+      <c r="K39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="4">
+        <v>0</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added my project counts
</commit_message>
<xml_diff>
--- a/COUNTforSENG.xlsx
+++ b/COUNTforSENG.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/loganpearce/Documents/GitHub/SENG300GROUP3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="75" documentId="13_ncr:1_{AC5BC41D-E805-2744-9E6E-4CED05FF385F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{0C6239DC-5F0B-48E9-B479-5C066B970766}"/>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="460" windowWidth="19940" windowHeight="19520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="29010" windowHeight="12960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179016"/>
+  <calcPr calcId="152511"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -28,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="83">
   <si>
     <t>Nested type count</t>
   </si>
@@ -244,12 +240,45 @@
   </si>
   <si>
     <t>Plaid App</t>
+  </si>
+  <si>
+    <t>Josh's Projects</t>
+  </si>
+  <si>
+    <t>jMonkeyEngine</t>
+  </si>
+  <si>
+    <t>libGDX</t>
+  </si>
+  <si>
+    <t>TEAMMATES</t>
+  </si>
+  <si>
+    <t>JUnit 4</t>
+  </si>
+  <si>
+    <t>Activiti</t>
+  </si>
+  <si>
+    <t>Kore</t>
+  </si>
+  <si>
+    <t>MyCollab</t>
+  </si>
+  <si>
+    <t>BioJava</t>
+  </si>
+  <si>
+    <t>Cryptomator</t>
+  </si>
+  <si>
+    <t>Java Google Maps</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -275,7 +304,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -283,11 +312,102 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -301,6 +421,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,26 +710,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L70"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8515625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="46.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.453125" customWidth="1"/>
-    <col min="3" max="3" width="13.31640625" customWidth="1"/>
-    <col min="4" max="4" width="20.71484375" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.98828125" customWidth="1"/>
-    <col min="7" max="7" width="13.31640625" customWidth="1"/>
-    <col min="8" max="8" width="15.2890625" customWidth="1"/>
+    <col min="1" max="1" width="46.875" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="13.375" customWidth="1"/>
+    <col min="4" max="4" width="20.75" customWidth="1"/>
+    <col min="5" max="5" width="11.75" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="13.375" customWidth="1"/>
+    <col min="8" max="8" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G1" t="s">
         <v>12</v>
       </c>
@@ -607,7 +737,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -639,7 +769,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -679,7 +809,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -718,7 +848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -758,7 +888,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -798,7 +928,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -838,7 +968,7 @@
         <v>1129</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -878,7 +1008,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -917,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -956,7 +1086,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -995,7 +1125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1034,12 +1164,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1087,13 +1217,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -1128,7 +1258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1163,7 +1293,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1198,7 +1328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1233,7 +1363,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1268,7 +1398,7 @@
         <v>1989</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1303,7 +1433,7 @@
         <v>7495</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1338,7 +1468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
@@ -1373,27 +1503,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1438,7 +1568,7 @@
         <v>10.256410256410255</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>36</v>
       </c>
@@ -1473,7 +1603,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1508,7 +1638,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
@@ -1543,7 +1673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -1578,7 +1708,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>3</v>
       </c>
@@ -1613,7 +1743,7 @@
         <v>1531</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>4</v>
       </c>
@@ -1648,7 +1778,7 @@
         <v>4809</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>27</v>
       </c>
@@ -1683,7 +1813,7 @@
         <v>1370</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>28</v>
       </c>
@@ -1718,7 +1848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>29</v>
       </c>
@@ -1753,7 +1883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>30</v>
       </c>
@@ -1788,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>31</v>
       </c>
@@ -1823,12 +1953,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>8</v>
       </c>
@@ -1873,7 +2003,7 @@
         <v>5.3559764859568908</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="74.25" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
@@ -1908,7 +2038,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +2073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
         <v>1</v>
       </c>
@@ -1978,7 +2108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>2</v>
       </c>
@@ -2013,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
         <v>58</v>
       </c>
@@ -2048,7 +2178,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>4</v>
       </c>
@@ -2083,7 +2213,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
         <v>59</v>
       </c>
@@ -2118,7 +2248,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>60</v>
       </c>
@@ -2153,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>61</v>
       </c>
@@ -2188,7 +2318,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -2223,7 +2353,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>1</v>
       </c>
@@ -2258,7 +2388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -2293,7 +2423,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
@@ -2328,7 +2458,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +2493,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>27</v>
       </c>
@@ -2398,7 +2528,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>28</v>
       </c>
@@ -2433,7 +2563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>29</v>
       </c>
@@ -2468,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>30</v>
       </c>
@@ -2503,7 +2633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>31</v>
       </c>
@@ -2538,12 +2668,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>8</v>
       </c>
@@ -2587,6 +2717,417 @@
         <f t="shared" si="3"/>
         <v>19.182389937106919</v>
       </c>
+    </row>
+    <row r="73" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F74" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G74" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="H74" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I74" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="J74" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K74" s="10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>0</v>
+      </c>
+      <c r="B75" s="11">
+        <v>789</v>
+      </c>
+      <c r="C75" s="11">
+        <v>467</v>
+      </c>
+      <c r="D75" s="11">
+        <v>10</v>
+      </c>
+      <c r="E75" s="2">
+        <v>600</v>
+      </c>
+      <c r="F75" s="11">
+        <v>36</v>
+      </c>
+      <c r="G75" s="12">
+        <v>225</v>
+      </c>
+      <c r="H75" s="11">
+        <v>613</v>
+      </c>
+      <c r="I75" s="12">
+        <v>76</v>
+      </c>
+      <c r="J75" s="11">
+        <v>10</v>
+      </c>
+      <c r="K75" s="13">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>1</v>
+      </c>
+      <c r="B76" s="11">
+        <v>0</v>
+      </c>
+      <c r="C76" s="11">
+        <v>0</v>
+      </c>
+      <c r="D76" s="11">
+        <v>0</v>
+      </c>
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+      <c r="F76" s="11">
+        <v>0</v>
+      </c>
+      <c r="G76" s="12">
+        <v>0</v>
+      </c>
+      <c r="H76" s="11">
+        <v>0</v>
+      </c>
+      <c r="I76" s="12">
+        <v>1</v>
+      </c>
+      <c r="J76" s="11">
+        <v>0</v>
+      </c>
+      <c r="K76" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>2</v>
+      </c>
+      <c r="B77" s="11">
+        <v>79</v>
+      </c>
+      <c r="C77" s="11">
+        <v>319</v>
+      </c>
+      <c r="D77" s="11">
+        <v>9</v>
+      </c>
+      <c r="E77" s="2">
+        <v>132</v>
+      </c>
+      <c r="F77" s="11">
+        <v>31</v>
+      </c>
+      <c r="G77" s="12">
+        <v>38</v>
+      </c>
+      <c r="H77" s="11">
+        <v>208</v>
+      </c>
+      <c r="I77" s="12">
+        <v>15</v>
+      </c>
+      <c r="J77" s="11">
+        <v>0</v>
+      </c>
+      <c r="K77" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="11">
+        <v>1686</v>
+      </c>
+      <c r="C78" s="11">
+        <v>2265</v>
+      </c>
+      <c r="D78" s="11">
+        <v>760</v>
+      </c>
+      <c r="E78" s="14">
+        <v>408</v>
+      </c>
+      <c r="F78" s="11">
+        <v>1949</v>
+      </c>
+      <c r="G78" s="12">
+        <v>225</v>
+      </c>
+      <c r="H78" s="11">
+        <v>1478</v>
+      </c>
+      <c r="I78" s="12">
+        <v>1268</v>
+      </c>
+      <c r="J78" s="11">
+        <v>79</v>
+      </c>
+      <c r="K78" s="11">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>4</v>
+      </c>
+      <c r="B79" s="11">
+        <v>13134</v>
+      </c>
+      <c r="C79" s="11">
+        <v>53529</v>
+      </c>
+      <c r="D79" s="11">
+        <v>1219</v>
+      </c>
+      <c r="E79" s="14">
+        <v>796</v>
+      </c>
+      <c r="F79" s="11">
+        <v>2269</v>
+      </c>
+      <c r="G79" s="12">
+        <v>996</v>
+      </c>
+      <c r="H79" s="11">
+        <v>4720</v>
+      </c>
+      <c r="I79" s="12">
+        <v>3567</v>
+      </c>
+      <c r="J79" s="11">
+        <v>71</v>
+      </c>
+      <c r="K79" s="11">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>27</v>
+      </c>
+      <c r="B80" s="11">
+        <v>2150</v>
+      </c>
+      <c r="C80" s="11">
+        <v>5288</v>
+      </c>
+      <c r="D80" s="11">
+        <v>1111</v>
+      </c>
+      <c r="E80" s="14">
+        <v>1856</v>
+      </c>
+      <c r="F80" s="11">
+        <v>1861</v>
+      </c>
+      <c r="G80" s="12">
+        <v>585</v>
+      </c>
+      <c r="H80" s="11">
+        <v>2764</v>
+      </c>
+      <c r="I80" s="12">
+        <v>1479</v>
+      </c>
+      <c r="J80" s="11">
+        <v>204</v>
+      </c>
+      <c r="K80" s="11">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>28</v>
+      </c>
+      <c r="B81" s="11">
+        <v>0</v>
+      </c>
+      <c r="C81" s="11">
+        <v>0</v>
+      </c>
+      <c r="D81" s="11">
+        <v>0</v>
+      </c>
+      <c r="E81" s="14">
+        <v>0</v>
+      </c>
+      <c r="F81" s="11">
+        <v>0</v>
+      </c>
+      <c r="G81" s="12">
+        <v>0</v>
+      </c>
+      <c r="H81" s="11">
+        <v>0</v>
+      </c>
+      <c r="I81" s="12">
+        <v>0</v>
+      </c>
+      <c r="J81" s="11">
+        <v>0</v>
+      </c>
+      <c r="K81" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+      <c r="B82" s="11">
+        <v>3</v>
+      </c>
+      <c r="C82" s="11">
+        <v>1</v>
+      </c>
+      <c r="D82" s="11">
+        <v>0</v>
+      </c>
+      <c r="E82" s="14">
+        <v>13</v>
+      </c>
+      <c r="F82" s="11">
+        <v>0</v>
+      </c>
+      <c r="G82" s="12">
+        <v>0</v>
+      </c>
+      <c r="H82" s="11">
+        <v>0</v>
+      </c>
+      <c r="I82" s="12">
+        <v>0</v>
+      </c>
+      <c r="J82" s="11">
+        <v>1</v>
+      </c>
+      <c r="K82" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>30</v>
+      </c>
+      <c r="B83" s="11">
+        <v>0</v>
+      </c>
+      <c r="C83" s="11">
+        <v>0</v>
+      </c>
+      <c r="D83" s="11">
+        <v>0</v>
+      </c>
+      <c r="E83" s="14">
+        <v>0</v>
+      </c>
+      <c r="F83" s="11">
+        <v>0</v>
+      </c>
+      <c r="G83" s="12">
+        <v>0</v>
+      </c>
+      <c r="H83" s="11">
+        <v>0</v>
+      </c>
+      <c r="I83" s="12">
+        <v>0</v>
+      </c>
+      <c r="J83" s="11">
+        <v>0</v>
+      </c>
+      <c r="K83" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>31</v>
+      </c>
+      <c r="B84" s="11">
+        <v>8</v>
+      </c>
+      <c r="C84" s="11">
+        <v>0</v>
+      </c>
+      <c r="D84" s="11">
+        <v>1</v>
+      </c>
+      <c r="E84" s="14">
+        <v>20</v>
+      </c>
+      <c r="F84" s="11">
+        <v>5</v>
+      </c>
+      <c r="G84" s="12">
+        <v>0</v>
+      </c>
+      <c r="H84" s="11">
+        <v>6</v>
+      </c>
+      <c r="I84" s="12">
+        <v>2</v>
+      </c>
+      <c r="J84" s="11">
+        <v>1</v>
+      </c>
+      <c r="K84" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>6</v>
+      </c>
+      <c r="B85" s="13"/>
+      <c r="C85" s="13"/>
+      <c r="D85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="13"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="15"/>
+      <c r="B86" s="16"/>
+      <c r="C86" s="16"/>
+      <c r="D86" s="16"/>
+      <c r="E86" s="15"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="15"/>
+      <c r="H86" s="16"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="16"/>
+      <c r="K86" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>